<commit_message>
update the gantt chart and backlog
</commit_message>
<xml_diff>
--- a/doc/WebMusic项目开发计划.xlsx
+++ b/doc/WebMusic项目开发计划.xlsx
@@ -1,20 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SueJane\Desktop\软工\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F42857-66BC-4716-86C3-97D42100C02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="17440"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表 1 - WebMusic项目开发计划" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <r>
       <t>WebMusic</t>
@@ -43,9 +59,6 @@
     <t>完成时间</t>
   </si>
   <si>
-    <t>备注</t>
-  </si>
-  <si>
     <r>
       <t>第</t>
     </r>
@@ -55,7 +68,7 @@
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>0</t>
     </r>
@@ -105,7 +118,7 @@
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>/</t>
     </r>
@@ -119,98 +132,6 @@
       </rPr>
       <t>资源获取</t>
     </r>
-  </si>
-  <si>
-    <t>任务布置会议</t>
-  </si>
-  <si>
-    <r>
-      <t>UI</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、资源、</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-        <charset val="134"/>
-      </rPr>
-      <t>api</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>会议</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>UI/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>音乐播放、检索</t>
-    </r>
-  </si>
-  <si>
-    <t>会议</t>
-  </si>
-  <si>
-    <r>
-      <t>UI/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>评论检索、标签</t>
-    </r>
-  </si>
-  <si>
-    <t>搜索模块会议</t>
-  </si>
-  <si>
-    <r>
-      <t>UI/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>用户登录设计</t>
-    </r>
-  </si>
-  <si>
-    <t>歌词设计会议</t>
   </si>
   <si>
     <t>歌词相关设计</t>
@@ -238,7 +159,7 @@
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>/</t>
     </r>
@@ -254,49 +175,7 @@
     </r>
   </si>
   <si>
-    <t>阶段总结会议</t>
-  </si>
-  <si>
-    <t>第一次迭代</t>
-  </si>
-  <si>
     <t>第一次迭代总结分析次会议</t>
-  </si>
-  <si>
-    <t>核心功能开发测试</t>
-  </si>
-  <si>
-    <r>
-      <t>核心测试与更新会议</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>核心测试与更新会议</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-        <charset val="134"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <t>最终迭代</t>
   </si>
   <si>
     <t>完善文档</t>
@@ -307,21 +186,112 @@
   <si>
     <t>完善项目</t>
   </si>
+  <si>
+    <t>音乐播放、检索api</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>首页</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>UI</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>UI/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音乐检索</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>api/获取评论</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>音乐播放功能实现</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户注册登录</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>评论检索、标签</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>评论UI设计</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>核心功能测试</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二次迭代总结分析</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>最终迭代</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成进度</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>api/获取歌词</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>api/获取热榜</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="177" formatCode="m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -332,14 +302,14 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue Medium"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -352,14 +322,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -373,158 +343,7 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -533,8 +352,51 @@
       <name val="宋体-简"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -555,192 +417,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFDEDE22"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFEAAF2A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -854,270 +554,89 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1129,106 +648,38 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -1297,17 +748,25 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFEAAF2A"/>
+      <color rgb="FFF5A70B"/>
+      <color rgb="FFDEDE22"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -1358,7 +817,23 @@
               </a:rPr>
               <a:t>标题</a:t>
             </a:r>
-            <a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1" forceAA="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:ln w="12700" cmpd="sng">
                 <a:solidFill>
                   <a:schemeClr val="accent1">
@@ -1367,19 +842,17 @@
                 </a:solidFill>
                 <a:prstDash val="solid"/>
               </a:ln>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1390,7 +863,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.189018410235405"/>
           <c:y val="0.121317806111207"/>
-          <c:w val="0.77468982630273"/>
+          <c:w val="0.77468982630272998"/>
           <c:h val="0.83821874702012"/>
         </c:manualLayout>
       </c:layout>
@@ -1402,15 +875,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>"开始时间"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>开始时间</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>开始时间</c:v>
           </c:tx>
           <c:spPr>
             <a:noFill/>
@@ -1425,7 +890,7 @@
               <c:idx val="19"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.00087746464333643"/>
+                  <c:x val="8.7746464333643003E-4"/>
                   <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
@@ -1437,39 +902,21 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-1E9C-4C33-B7CF-4B0CC20B812C}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="20"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
+                  <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:pPr defTabSz="914400">
-                      <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:ln w="12700" cmpd="sng">
-                          <a:solidFill>
-                            <a:schemeClr val="accent1">
-                              <a:shade val="50000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                          <a:prstDash val="solid"/>
-                        </a:ln>
-                        <a:solidFill>
-                          <a:schemeClr val="bg1"/>
-                        </a:solidFill>
-                        <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
-                      </a:defRPr>
-                    </a:pPr>
                     <a:r>
-                      <a:rPr>
+                      <a:rPr lang="en-US" altLang="zh-CN">
                         <a:ln w="12700" cmpd="sng">
                           <a:solidFill>
                             <a:schemeClr val="accent1">
@@ -1479,10 +926,49 @@
                           <a:prstDash val="solid"/>
                         </a:ln>
                       </a:rPr>
-                      <a:t>11月27日</a:t>
+                      <a:t>11</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr>
+                      <a:rPr lang="zh-CN" altLang="en-US">
+                        <a:ln w="12700" cmpd="sng">
+                          <a:solidFill>
+                            <a:schemeClr val="accent1">
+                              <a:shade val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:prstDash val="solid"/>
+                        </a:ln>
+                      </a:rPr>
+                      <a:t>月</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" altLang="zh-CN">
+                        <a:ln w="12700" cmpd="sng">
+                          <a:solidFill>
+                            <a:schemeClr val="accent1">
+                              <a:shade val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:prstDash val="solid"/>
+                        </a:ln>
+                      </a:rPr>
+                      <a:t>27</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="zh-CN" altLang="en-US">
+                        <a:ln w="12700" cmpd="sng">
+                          <a:solidFill>
+                            <a:schemeClr val="accent1">
+                              <a:shade val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:prstDash val="solid"/>
+                        </a:ln>
+                      </a:rPr>
+                      <a:t>日</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="zh-CN" altLang="en-US">
                         <a:ln w="12700" cmpd="sng">
                           <a:noFill/>
                           <a:prstDash val="solid"/>
@@ -1490,12 +976,6 @@
                       </a:rPr>
                       <a:t>日</a:t>
                     </a:r>
-                    <a:endParaRPr>
-                      <a:ln w="12700" cmpd="sng">
-                        <a:noFill/>
-                        <a:prstDash val="solid"/>
-                      </a:ln>
-                    </a:endParaRPr>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1507,10 +987,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-1E9C-4C33-B7CF-4B0CC20B812C}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1540,6 +1024,7 @@
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1552,100 +1037,82 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'工作表 1 - WebMusic项目开发计划'!$A$3:$A$26</c:f>
+              <c:f>'工作表 1 - WebMusic项目开发计划'!$A$3:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
-                <c:pt idx="0" c:formatCode="@">
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
                   <c:v>第0次会议</c:v>
                 </c:pt>
-                <c:pt idx="1" c:formatCode="@">
+                <c:pt idx="1">
                   <c:v>demo开发</c:v>
                 </c:pt>
-                <c:pt idx="2" c:formatCode="@">
+                <c:pt idx="2">
                   <c:v>UI设计/资源获取</c:v>
                 </c:pt>
-                <c:pt idx="3" c:formatCode="@">
-                  <c:v>任务布置会议</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="@">
-                  <c:v>UI、资源、api会议</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="@">
-                  <c:v>UI/音乐播放、检索</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="@">
-                  <c:v>会议</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="@">
-                  <c:v>UI/评论检索、标签</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="@">
-                  <c:v>搜索模块会议</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="@">
-                  <c:v>UI/用户登录设计</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="@">
-                  <c:v>歌词设计会议</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="@">
+                <c:pt idx="3">
+                  <c:v>音乐播放、检索api</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>首页UI</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>UI/音乐检索</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>api/获取评论</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>音乐播放功能实现</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>api/获取歌词</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>api/获取热榜</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>用户注册登录</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>评论UI设计</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>评论检索、标签</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>第一次迭代总结分析次会议</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>歌词相关设计</c:v>
                 </c:pt>
-                <c:pt idx="12" c:formatCode="@">
+                <c:pt idx="15">
                   <c:v>优化界面、总结分析会议</c:v>
                 </c:pt>
-                <c:pt idx="13" c:formatCode="@">
+                <c:pt idx="16">
                   <c:v>UI优化/词义分析</c:v>
                 </c:pt>
-                <c:pt idx="14" c:formatCode="@">
-                  <c:v>阶段总结会议</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="@">
-                  <c:v>第一次迭代</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="@">
-                  <c:v>第一次迭代总结分析次会议</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="@">
-                  <c:v>核心功能开发测试</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="@">
-                  <c:v>核心测试与更新会议1</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="@">
-                  <c:v>核心测试与更新会议2</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="@">
+                <c:pt idx="17">
+                  <c:v>核心功能测试</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>第二次迭代总结分析</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>最终迭代</c:v>
                 </c:pt>
-                <c:pt idx="21" c:formatCode="@">
+                <c:pt idx="20">
                   <c:v>完善文档</c:v>
                 </c:pt>
-                <c:pt idx="22" c:formatCode="@">
+                <c:pt idx="21">
                   <c:v>总结会议</c:v>
                 </c:pt>
-                <c:pt idx="23" c:formatCode="@">
+                <c:pt idx="22">
                   <c:v>完善项目</c:v>
                 </c:pt>
               </c:strCache>
@@ -1653,10 +1120,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'工作表 1 - WebMusic项目开发计划'!$B$3:$B$26</c:f>
+              <c:f>'工作表 1 - WebMusic项目开发计划'!$B$3:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日";@</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>44823</c:v>
                 </c:pt>
@@ -1667,85 +1134,79 @@
                   <c:v>44823</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44830</c:v>
+                  <c:v>44843</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44836</c:v>
+                  <c:v>44844</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44836</c:v>
+                  <c:v>44851</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44843</c:v>
+                  <c:v>44851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44843</c:v>
+                  <c:v>44859</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44850</c:v>
+                  <c:v>44859</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44850</c:v>
+                  <c:v>44859</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44857</c:v>
+                  <c:v>44865</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44857</c:v>
+                  <c:v>44872</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44864</c:v>
+                  <c:v>44872</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44864</c:v>
+                  <c:v>44878</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44871</c:v>
+                  <c:v>44878</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>44872</c:v>
+                  <c:v>44886</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>44878</c:v>
+                  <c:v>44887</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>44878</c:v>
+                  <c:v>44891</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44885</c:v>
+                  <c:v>44893</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44892</c:v>
+                  <c:v>44896</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44892</c:v>
+                  <c:v>44896</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44892</c:v>
+                  <c:v>44900</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44899</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44899</c:v>
+                  <c:v>44903</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1E9C-4C33-B7CF-4B0CC20B812C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>"持续时间"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>持续时间</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>持续时间</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1758,7 +1219,6 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1788,6 +1248,7 @@
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1800,100 +1261,82 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'工作表 1 - WebMusic项目开发计划'!$A$3:$A$26</c:f>
+              <c:f>'工作表 1 - WebMusic项目开发计划'!$A$3:$A$25</c:f>
               <c:strCache>
-                <c:ptCount val="24"/>
-                <c:pt idx="0" c:formatCode="@">
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
                   <c:v>第0次会议</c:v>
                 </c:pt>
-                <c:pt idx="1" c:formatCode="@">
+                <c:pt idx="1">
                   <c:v>demo开发</c:v>
                 </c:pt>
-                <c:pt idx="2" c:formatCode="@">
+                <c:pt idx="2">
                   <c:v>UI设计/资源获取</c:v>
                 </c:pt>
-                <c:pt idx="3" c:formatCode="@">
-                  <c:v>任务布置会议</c:v>
-                </c:pt>
-                <c:pt idx="4" c:formatCode="@">
-                  <c:v>UI、资源、api会议</c:v>
-                </c:pt>
-                <c:pt idx="5" c:formatCode="@">
-                  <c:v>UI/音乐播放、检索</c:v>
-                </c:pt>
-                <c:pt idx="6" c:formatCode="@">
-                  <c:v>会议</c:v>
-                </c:pt>
-                <c:pt idx="7" c:formatCode="@">
-                  <c:v>UI/评论检索、标签</c:v>
-                </c:pt>
-                <c:pt idx="8" c:formatCode="@">
-                  <c:v>搜索模块会议</c:v>
-                </c:pt>
-                <c:pt idx="9" c:formatCode="@">
-                  <c:v>UI/用户登录设计</c:v>
-                </c:pt>
-                <c:pt idx="10" c:formatCode="@">
-                  <c:v>歌词设计会议</c:v>
-                </c:pt>
-                <c:pt idx="11" c:formatCode="@">
+                <c:pt idx="3">
+                  <c:v>音乐播放、检索api</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>首页UI</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>UI/音乐检索</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>api/获取评论</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>音乐播放功能实现</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>api/获取歌词</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>api/获取热榜</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>用户注册登录</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>评论UI设计</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>评论检索、标签</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>第一次迭代总结分析次会议</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>歌词相关设计</c:v>
                 </c:pt>
-                <c:pt idx="12" c:formatCode="@">
+                <c:pt idx="15">
                   <c:v>优化界面、总结分析会议</c:v>
                 </c:pt>
-                <c:pt idx="13" c:formatCode="@">
+                <c:pt idx="16">
                   <c:v>UI优化/词义分析</c:v>
                 </c:pt>
-                <c:pt idx="14" c:formatCode="@">
-                  <c:v>阶段总结会议</c:v>
-                </c:pt>
-                <c:pt idx="15" c:formatCode="@">
-                  <c:v>第一次迭代</c:v>
-                </c:pt>
-                <c:pt idx="16" c:formatCode="@">
-                  <c:v>第一次迭代总结分析次会议</c:v>
-                </c:pt>
-                <c:pt idx="17" c:formatCode="@">
-                  <c:v>核心功能开发测试</c:v>
-                </c:pt>
-                <c:pt idx="18" c:formatCode="@">
-                  <c:v>核心测试与更新会议1</c:v>
-                </c:pt>
-                <c:pt idx="19" c:formatCode="@">
-                  <c:v>核心测试与更新会议2</c:v>
-                </c:pt>
-                <c:pt idx="20" c:formatCode="@">
+                <c:pt idx="17">
+                  <c:v>核心功能测试</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>第二次迭代总结分析</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>最终迭代</c:v>
                 </c:pt>
-                <c:pt idx="21" c:formatCode="@">
+                <c:pt idx="20">
                   <c:v>完善文档</c:v>
                 </c:pt>
-                <c:pt idx="22" c:formatCode="@">
+                <c:pt idx="21">
                   <c:v>总结会议</c:v>
                 </c:pt>
-                <c:pt idx="23" c:formatCode="@">
+                <c:pt idx="22">
                   <c:v>完善项目</c:v>
                 </c:pt>
               </c:strCache>
@@ -1901,10 +1344,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'工作表 1 - WebMusic项目开发计划'!$C$3:$C$26</c:f>
+              <c:f>'工作表 1 - WebMusic项目开发计划'!$C$3:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0_ </c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1915,71 +1358,73 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>14</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1E9C-4C33-B7CF-4B0CC20B812C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2040,6 +1485,7 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="923305182"/>
@@ -2094,6 +1540,7 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="970757635"/>
@@ -2162,6 +1609,7 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
@@ -2189,10 +1637,10 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2223,6 +1671,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2266,6 +1715,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="7" charset="0"/>
         </a:defRPr>
       </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2820,28 +2270,34 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1143635</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1120775</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
+      <xdr:rowOff>188105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>604520</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>187325</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>234460</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="图表 3"/>
+        <xdr:cNvPr id="4" name="图表 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5056505" y="140970"/>
-        <a:ext cx="12250420" cy="10441305"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3052,7 +2508,7 @@
           <a:miter lim="400000"/>
         </a:ln>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3335,7 +2791,7 @@
           <a:miter lim="400000"/>
         </a:ln>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3611,7 +3067,7 @@
           <a:miter lim="400000"/>
         </a:ln>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3884,6 +3340,7 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -4140,507 +3597,563 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3303571428571" defaultRowHeight="19.9" customHeight="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.3214285714286" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3482142857143" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.3482142857143" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.3482142857143" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="16.3482142857143" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="16.33203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20" customHeight="1" spans="1:7">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
-    <row r="2" ht="20" customHeight="1" spans="1:7">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="3" ht="20" customHeight="1" spans="1:7">
-      <c r="A3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>44823</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="11">
         <v>1</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="12">
         <f>B3+C3</f>
         <v>44824</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
+      <c r="E3" s="29">
+        <v>1</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
     </row>
-    <row r="4" ht="20" customHeight="1" spans="1:7">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="14">
+        <v>44823</v>
+      </c>
+      <c r="C4" s="15">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12">
+        <f>B4+C4</f>
+        <v>44826</v>
+      </c>
+      <c r="E4" s="29">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B5" s="14">
         <v>44823</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C5" s="15">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12">
+        <f>B5+C5</f>
+        <v>44830</v>
+      </c>
+      <c r="E5" s="29">
+        <v>1</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="14">
+        <v>44843</v>
+      </c>
+      <c r="C6" s="15">
+        <v>14</v>
+      </c>
+      <c r="D6" s="12">
+        <f>B6+C6</f>
+        <v>44857</v>
+      </c>
+      <c r="E6" s="29">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="14">
+        <v>44844</v>
+      </c>
+      <c r="C7" s="15">
+        <v>7</v>
+      </c>
+      <c r="D7" s="12">
+        <f>B7+C7</f>
+        <v>44851</v>
+      </c>
+      <c r="E7" s="29">
+        <v>1</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+    </row>
+    <row r="8" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A8" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="14">
+        <v>44851</v>
+      </c>
+      <c r="C8" s="15">
+        <v>10</v>
+      </c>
+      <c r="D8" s="12">
+        <f>B8+C8</f>
+        <v>44861</v>
+      </c>
+      <c r="E8" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A9" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="14">
+        <v>44851</v>
+      </c>
+      <c r="C9" s="15">
+        <v>7</v>
+      </c>
+      <c r="D9" s="12">
+        <f>B9+C9</f>
+        <v>44858</v>
+      </c>
+      <c r="E9" s="29">
+        <v>1</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+    </row>
+    <row r="10" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A10" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="14">
+        <v>44859</v>
+      </c>
+      <c r="C10" s="15">
+        <v>10</v>
+      </c>
+      <c r="D10" s="12">
+        <f>B10+C10</f>
+        <v>44869</v>
+      </c>
+      <c r="E10" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+    </row>
+    <row r="11" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A11" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="14">
+        <v>44859</v>
+      </c>
+      <c r="C11" s="15">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12">
+        <f>B11+C11</f>
+        <v>44866</v>
+      </c>
+      <c r="E11" s="31">
+        <v>0.7</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+    </row>
+    <row r="12" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A12" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="14">
+        <v>44859</v>
+      </c>
+      <c r="C12" s="15">
+        <v>7</v>
+      </c>
+      <c r="D12" s="12">
+        <f>B12+C12</f>
+        <v>44866</v>
+      </c>
+      <c r="E12" s="33">
+        <v>1</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="14">
+        <v>44865</v>
+      </c>
+      <c r="C13" s="15">
+        <v>7</v>
+      </c>
+      <c r="D13" s="12">
+        <f>B13+C13</f>
+        <v>44872</v>
+      </c>
+      <c r="E13" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A14" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="14">
+        <v>44872</v>
+      </c>
+      <c r="C14" s="15">
+        <v>7</v>
+      </c>
+      <c r="D14" s="12">
+        <f>B14+C14</f>
+        <v>44879</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="14">
+        <v>44872</v>
+      </c>
+      <c r="C15" s="15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="12">
+        <f>B15+C15</f>
+        <v>44886</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="14">
+        <v>44878</v>
+      </c>
+      <c r="C16" s="15">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12">
+        <f>B16+C16</f>
+        <v>44879</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="14">
+        <v>44878</v>
+      </c>
+      <c r="C17" s="15">
+        <v>7</v>
+      </c>
+      <c r="D17" s="12">
+        <f>B17+C17</f>
+        <v>44885</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A18" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="14">
+        <v>44886</v>
+      </c>
+      <c r="C18" s="15">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12">
+        <f>B18+C18</f>
+        <v>44887</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A19" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="14">
+        <v>44887</v>
+      </c>
+      <c r="C19" s="15">
+        <v>7</v>
+      </c>
+      <c r="D19" s="12">
+        <f>B19+C19</f>
+        <v>44894</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A20" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="14">
+        <v>44891</v>
+      </c>
+      <c r="C20" s="15">
         <v>3</v>
       </c>
-      <c r="D4" s="15">
-        <f t="shared" ref="D4:D26" si="0">B4+C4</f>
-        <v>44826</v>
-      </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D20" s="12">
+        <f>B20+C20</f>
+        <v>44894</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
     </row>
-    <row r="5" ht="20" customHeight="1" spans="1:7">
-      <c r="A5" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="17">
+    <row r="21" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A21" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="14">
+        <v>44893</v>
+      </c>
+      <c r="C21" s="15">
+        <v>1</v>
+      </c>
+      <c r="D21" s="12">
+        <f>B21+C21</f>
+        <v>44894</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A22" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="14">
+        <v>44896</v>
+      </c>
+      <c r="C22" s="15">
+        <v>7</v>
+      </c>
+      <c r="D22" s="12">
+        <f>B22+C22</f>
+        <v>44903</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="14">
+        <v>44896</v>
+      </c>
+      <c r="C23" s="15">
+        <v>7</v>
+      </c>
+      <c r="D23" s="12">
+        <f>B23+C23</f>
+        <v>44903</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+    </row>
+    <row r="24" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A24" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="14">
+        <v>44900</v>
+      </c>
+      <c r="C24" s="15">
+        <v>1</v>
+      </c>
+      <c r="D24" s="12">
+        <f>B24+C24</f>
+        <v>44901</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+    </row>
+    <row r="25" spans="1:7" ht="19.95" customHeight="1" thickBot="1">
+      <c r="A25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="14">
+        <v>44903</v>
+      </c>
+      <c r="C25" s="15">
+        <v>5</v>
+      </c>
+      <c r="D25" s="12">
+        <f>B25+C25</f>
+        <v>44908</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+    </row>
+    <row r="28" spans="1:7" ht="19.95" customHeight="1">
+      <c r="B28" s="17">
+        <f>MIN(B3:B25)</f>
         <v>44823</v>
       </c>
-      <c r="C5" s="18">
-        <v>7</v>
-      </c>
-      <c r="D5" s="15">
-        <f t="shared" si="0"/>
-        <v>44830</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
     </row>
-    <row r="6" ht="20" customHeight="1" spans="1:7">
-      <c r="A6" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="17">
-        <v>44830</v>
-      </c>
-      <c r="C6" s="18">
-        <v>1</v>
-      </c>
-      <c r="D6" s="15">
-        <f t="shared" si="0"/>
-        <v>44831</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-    </row>
-    <row r="7" ht="20" customHeight="1" spans="1:7">
-      <c r="A7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="17">
-        <v>44836</v>
-      </c>
-      <c r="C7" s="18">
-        <v>1</v>
-      </c>
-      <c r="D7" s="15">
-        <f t="shared" si="0"/>
-        <v>44837</v>
-      </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-    </row>
-    <row r="8" ht="20" customHeight="1" spans="1:7">
-      <c r="A8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="17">
-        <v>44836</v>
-      </c>
-      <c r="C8" s="18">
-        <v>7</v>
-      </c>
-      <c r="D8" s="15">
-        <f t="shared" si="0"/>
-        <v>44843</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-    </row>
-    <row r="9" ht="20" customHeight="1" spans="1:7">
-      <c r="A9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="17">
-        <v>44843</v>
-      </c>
-      <c r="C9" s="18">
-        <v>1</v>
-      </c>
-      <c r="D9" s="15">
-        <f t="shared" si="0"/>
-        <v>44844</v>
-      </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-    </row>
-    <row r="10" ht="20" customHeight="1" spans="1:7">
-      <c r="A10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="17">
-        <v>44843</v>
-      </c>
-      <c r="C10" s="18">
-        <v>14</v>
-      </c>
-      <c r="D10" s="15">
-        <f t="shared" si="0"/>
-        <v>44857</v>
-      </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-    </row>
-    <row r="11" ht="20" customHeight="1" spans="1:7">
-      <c r="A11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="17">
-        <v>44850</v>
-      </c>
-      <c r="C11" s="18">
-        <v>1</v>
-      </c>
-      <c r="D11" s="15">
-        <f t="shared" si="0"/>
-        <v>44851</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-    </row>
-    <row r="12" ht="20" customHeight="1" spans="1:7">
-      <c r="A12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="17">
-        <v>44850</v>
-      </c>
-      <c r="C12" s="18">
-        <v>7</v>
-      </c>
-      <c r="D12" s="15">
-        <f t="shared" si="0"/>
-        <v>44857</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-    </row>
-    <row r="13" ht="20" customHeight="1" spans="1:7">
-      <c r="A13" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="17">
-        <v>44857</v>
-      </c>
-      <c r="C13" s="18">
-        <v>1</v>
-      </c>
-      <c r="D13" s="15">
-        <f t="shared" si="0"/>
-        <v>44858</v>
-      </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-    </row>
-    <row r="14" ht="20" customHeight="1" spans="1:7">
-      <c r="A14" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="17">
-        <v>44857</v>
-      </c>
-      <c r="C14" s="18">
-        <v>7</v>
-      </c>
-      <c r="D14" s="15">
-        <f t="shared" si="0"/>
-        <v>44864</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-    </row>
-    <row r="15" ht="20" customHeight="1" spans="1:7">
-      <c r="A15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="17">
-        <v>44864</v>
-      </c>
-      <c r="C15" s="18">
-        <v>1</v>
-      </c>
-      <c r="D15" s="15">
-        <f t="shared" si="0"/>
-        <v>44865</v>
-      </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-    </row>
-    <row r="16" ht="20" customHeight="1" spans="1:7">
-      <c r="A16" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="17">
-        <v>44864</v>
-      </c>
-      <c r="C16" s="18">
-        <v>7</v>
-      </c>
-      <c r="D16" s="15">
-        <f t="shared" si="0"/>
-        <v>44871</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-    </row>
-    <row r="17" ht="20" customHeight="1" spans="1:7">
-      <c r="A17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="17">
-        <v>44871</v>
-      </c>
-      <c r="C17" s="18">
-        <v>1</v>
-      </c>
-      <c r="D17" s="15">
-        <f t="shared" si="0"/>
-        <v>44872</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-    </row>
-    <row r="18" ht="20" customHeight="1" spans="1:7">
-      <c r="A18" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="17">
-        <v>44872</v>
-      </c>
-      <c r="C18" s="18">
-        <v>3</v>
-      </c>
-      <c r="D18" s="15">
-        <f t="shared" si="0"/>
-        <v>44875</v>
-      </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-    </row>
-    <row r="19" ht="20" customHeight="1" spans="1:7">
-      <c r="A19" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="17">
-        <v>44878</v>
-      </c>
-      <c r="C19" s="18">
-        <v>1</v>
-      </c>
-      <c r="D19" s="15">
-        <f t="shared" si="0"/>
-        <v>44879</v>
-      </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-    </row>
-    <row r="20" ht="20" customHeight="1" spans="1:7">
-      <c r="A20" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="17">
-        <v>44878</v>
-      </c>
-      <c r="C20" s="18">
-        <v>14</v>
-      </c>
-      <c r="D20" s="15">
-        <f t="shared" si="0"/>
-        <v>44892</v>
-      </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-    </row>
-    <row r="21" ht="20" customHeight="1" spans="1:7">
-      <c r="A21" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="17">
-        <v>44885</v>
-      </c>
-      <c r="C21" s="18">
-        <v>1</v>
-      </c>
-      <c r="D21" s="15">
-        <f t="shared" si="0"/>
-        <v>44886</v>
-      </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-    </row>
-    <row r="22" ht="20" customHeight="1" spans="1:7">
-      <c r="A22" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="17">
-        <v>44892</v>
-      </c>
-      <c r="C22" s="18">
-        <v>1</v>
-      </c>
-      <c r="D22" s="15">
-        <f t="shared" si="0"/>
-        <v>44893</v>
-      </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-    </row>
-    <row r="23" ht="20" customHeight="1" spans="1:7">
-      <c r="A23" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="17">
-        <v>44892</v>
-      </c>
-      <c r="C23" s="18">
-        <v>7</v>
-      </c>
-      <c r="D23" s="15">
-        <f t="shared" si="0"/>
-        <v>44899</v>
-      </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-    </row>
-    <row r="24" ht="20" customHeight="1" spans="1:7">
-      <c r="A24" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="17">
-        <v>44892</v>
-      </c>
-      <c r="C24" s="18">
-        <v>7</v>
-      </c>
-      <c r="D24" s="15">
-        <f t="shared" si="0"/>
-        <v>44899</v>
-      </c>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-    </row>
-    <row r="25" ht="20" customHeight="1" spans="1:7">
-      <c r="A25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="17">
-        <v>44899</v>
-      </c>
-      <c r="C25" s="18">
-        <v>1</v>
-      </c>
-      <c r="D25" s="15">
-        <f t="shared" si="0"/>
-        <v>44900</v>
-      </c>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-    </row>
-    <row r="26" ht="20" customHeight="1" spans="1:7">
-      <c r="A26" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="17">
-        <v>44899</v>
-      </c>
-      <c r="C26" s="18">
-        <v>7</v>
-      </c>
-      <c r="D26" s="15">
-        <f t="shared" si="0"/>
-        <v>44906</v>
-      </c>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-    </row>
-    <row r="29" customHeight="1" spans="2:2">
-      <c r="B29" s="20">
-        <f>MIN(B3:B26)</f>
-        <v>44823</v>
-      </c>
-    </row>
-    <row r="30" customHeight="1" spans="2:2">
-      <c r="B30" s="20">
-        <f>MAX(B26)</f>
-        <v>44899</v>
+    <row r="29" spans="1:7" ht="19.95" customHeight="1">
+      <c r="B29" s="17">
+        <f>MAX(B25)</f>
+        <v>44903</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup paperSize="1" scale="72" orientation="portrait" useFirstPageNumber="1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="0.5"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="percentile" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>